<commit_message>
copying data in table format
</commit_message>
<xml_diff>
--- a/Excel-Documents/WBManifestTable_1706103354202.xlsx
+++ b/Excel-Documents/WBManifestTable_1706103354202.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3800" yWindow="3800" windowWidth="21600" windowHeight="12670" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="760" yWindow="760" windowWidth="21600" windowHeight="12670" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="FedEx Air Ops Workbench Report" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="sort_times" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FedEx Air Ops Workbench Report" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sort_times" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FedEx Air Ops Workbench Report'!$A$4:$N$4</definedName>
@@ -172,6 +172,26 @@
       <left/>
       <right/>
       <top style="medium">
+        <color indexed="54"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="54"/>
+      </right>
+      <top style="medium">
+        <color indexed="54"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
         <color indexed="41"/>
       </top>
       <bottom/>
@@ -189,26 +209,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="54"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="54"/>
-      </right>
-      <top style="medium">
-        <color indexed="54"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color rgb="00000000"/>
       </left>
@@ -221,7 +221,6 @@
       <bottom style="medium">
         <color rgb="00000000"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -238,22 +237,90 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -584,132 +651,132 @@
   </cols>
   <sheetData>
     <row r="1" ht="50" customHeight="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>FedEx Air Ops Workbench Report</t>
         </is>
       </c>
-      <c r="B1" s="5" t="n"/>
-      <c r="C1" s="5" t="n"/>
-      <c r="D1" s="5" t="n"/>
-      <c r="E1" s="5" t="n"/>
-      <c r="F1" s="5" t="n"/>
-      <c r="G1" s="5" t="n"/>
-      <c r="H1" s="5" t="n"/>
-      <c r="I1" s="5" t="n"/>
-      <c r="J1" s="5" t="n"/>
-      <c r="K1" s="5" t="n"/>
-      <c r="L1" s="5" t="n"/>
-      <c r="M1" s="5" t="n"/>
-      <c r="N1" s="6" t="n"/>
+      <c r="B1" s="8" t="n"/>
+      <c r="C1" s="8" t="n"/>
+      <c r="D1" s="8" t="n"/>
+      <c r="E1" s="8" t="n"/>
+      <c r="F1" s="8" t="n"/>
+      <c r="G1" s="8" t="n"/>
+      <c r="H1" s="8" t="n"/>
+      <c r="I1" s="8" t="n"/>
+      <c r="J1" s="8" t="n"/>
+      <c r="K1" s="8" t="n"/>
+      <c r="L1" s="8" t="n"/>
+      <c r="M1" s="8" t="n"/>
+      <c r="N1" s="9" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="inlineStr">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>Requested by: Wessel, Nicole(5287297) On 24Jan2024 08:35:54</t>
         </is>
       </c>
-      <c r="B2" s="8" t="n"/>
-      <c r="C2" s="8" t="n"/>
-      <c r="D2" s="8" t="n"/>
-      <c r="E2" s="8" t="n"/>
-      <c r="F2" s="8" t="n"/>
-      <c r="G2" s="8" t="n"/>
-      <c r="H2" s="8" t="n"/>
-      <c r="I2" s="8" t="n"/>
-      <c r="J2" s="8" t="n"/>
-      <c r="K2" s="8" t="n"/>
-      <c r="L2" s="8" t="n"/>
-      <c r="M2" s="8" t="n"/>
-      <c r="N2" s="9" t="n"/>
+      <c r="B2" s="5" t="n"/>
+      <c r="C2" s="5" t="n"/>
+      <c r="D2" s="5" t="n"/>
+      <c r="E2" s="5" t="n"/>
+      <c r="F2" s="5" t="n"/>
+      <c r="G2" s="5" t="n"/>
+      <c r="H2" s="5" t="n"/>
+      <c r="I2" s="5" t="n"/>
+      <c r="J2" s="5" t="n"/>
+      <c r="K2" s="5" t="n"/>
+      <c r="L2" s="5" t="n"/>
+      <c r="M2" s="5" t="n"/>
+      <c r="N2" s="6" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="inlineStr">
+      <c r="A3" s="4" t="inlineStr">
         <is>
           <t>1460-20,LEG 1,N733FD,0055,MEM-CVG,PRA#80263,VSL:305306495876</t>
         </is>
       </c>
-      <c r="B3" s="8" t="n"/>
-      <c r="C3" s="8" t="n"/>
-      <c r="D3" s="8" t="n"/>
-      <c r="E3" s="8" t="n"/>
-      <c r="F3" s="8" t="n"/>
-      <c r="G3" s="8" t="n"/>
-      <c r="H3" s="8" t="n"/>
-      <c r="I3" s="8" t="n"/>
-      <c r="J3" s="8" t="n"/>
-      <c r="K3" s="8" t="n"/>
-      <c r="L3" s="8" t="n"/>
-      <c r="M3" s="8" t="n"/>
-      <c r="N3" s="9" t="n"/>
+      <c r="B3" s="5" t="n"/>
+      <c r="C3" s="5" t="n"/>
+      <c r="D3" s="5" t="n"/>
+      <c r="E3" s="5" t="n"/>
+      <c r="F3" s="5" t="n"/>
+      <c r="G3" s="5" t="n"/>
+      <c r="H3" s="5" t="n"/>
+      <c r="I3" s="5" t="n"/>
+      <c r="J3" s="5" t="n"/>
+      <c r="K3" s="5" t="n"/>
+      <c r="L3" s="5" t="n"/>
+      <c r="M3" s="5" t="n"/>
+      <c r="N3" s="6" t="n"/>
     </row>
     <row r="4" ht="40" customHeight="1">
-      <c r="A4" s="7" t="inlineStr">
+      <c r="A4" s="4" t="inlineStr">
         <is>
           <t>Pos</t>
         </is>
       </c>
-      <c r="B4" s="7" t="inlineStr">
+      <c r="B4" s="4" t="inlineStr">
         <is>
           <t>ULD</t>
         </is>
       </c>
-      <c r="C4" s="7" t="inlineStr">
+      <c r="C4" s="4" t="inlineStr">
         <is>
           <t>CD</t>
         </is>
       </c>
-      <c r="D4" s="7" t="inlineStr">
+      <c r="D4" s="4" t="inlineStr">
         <is>
           <t>Weight</t>
         </is>
       </c>
-      <c r="E4" s="7" t="inlineStr">
+      <c r="E4" s="4" t="inlineStr">
         <is>
           <t>Dest</t>
         </is>
       </c>
-      <c r="F4" s="7" t="inlineStr">
+      <c r="F4" s="4" t="inlineStr">
         <is>
           <t>CB</t>
         </is>
       </c>
-      <c r="G4" s="7" t="inlineStr">
+      <c r="G4" s="4" t="inlineStr">
         <is>
           <t>Service CD</t>
         </is>
       </c>
-      <c r="H4" s="7" t="inlineStr">
+      <c r="H4" s="4" t="inlineStr">
         <is>
           <t>Load CD</t>
         </is>
       </c>
-      <c r="I4" s="7" t="inlineStr">
+      <c r="I4" s="4" t="inlineStr">
         <is>
           <t>Pkg Dests</t>
         </is>
       </c>
-      <c r="J4" s="7" t="inlineStr">
+      <c r="J4" s="4" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
       </c>
-      <c r="K4" s="7" t="inlineStr">
+      <c r="K4" s="4" t="inlineStr">
         <is>
           <t>CONS#</t>
         </is>
       </c>
-      <c r="L4" s="7" t="inlineStr">
+      <c r="L4" s="4" t="inlineStr">
         <is>
           <t>Hgt</t>
         </is>
       </c>
-      <c r="M4" s="7" t="inlineStr">
+      <c r="M4" s="4" t="inlineStr">
         <is>
           <t>Src</t>
         </is>
       </c>
-      <c r="N4" s="7" t="inlineStr">
+      <c r="N4" s="4" t="inlineStr">
         <is>
           <t>Route</t>
         </is>
@@ -3434,9 +3501,9 @@
   </sheetData>
   <autoFilter ref="A4:N4"/>
   <mergeCells count="3">
+    <mergeCell ref="A3:N3"/>
+    <mergeCell ref="A2:N2"/>
     <mergeCell ref="A1:N1"/>
-    <mergeCell ref="A2:N2"/>
-    <mergeCell ref="A3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>